<commit_message>
them view detail sheet
</commit_message>
<xml_diff>
--- a/Test scenario & Test case/TestCase-Openmrs.xlsx
+++ b/Test scenario & Test case/TestCase-Openmrs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPTU\Ky5\SWT301\Nhom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPTU\Ky5\SWT301\Nhom\Git\OpenMRSTesting-SWT301\Test scenario &amp; Test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD84C44-A38A-42BA-BAC9-BDE0A5536CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BEBA3F-AA08-4372-85F4-BB8D50D0C5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Test Steps</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Search Field: "2323"</t>
   </si>
   <si>
-    <t>Search Field: "100"</t>
-  </si>
-  <si>
     <t>Search Field: " 100 "</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>Verify the user can see detailed information about the patient</t>
-  </si>
-  <si>
-    <t>Click on the patient that the user wants to see the patient details</t>
   </si>
   <si>
     <t>The system successfully displays patient details</t>
@@ -303,6 +297,13 @@
   <si>
     <t>Username: admin111
 Password: Admin123</t>
+  </si>
+  <si>
+    <t>1. Enter a value in Search Field
+2. Click on the patient that the user wants to see the patient details</t>
+  </si>
+  <si>
+    <t>Search Field: "100P9K"</t>
   </si>
 </sst>
 </file>
@@ -895,7 +896,7 @@
   </sheetPr>
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
@@ -959,28 +960,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="E2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -1001,28 +1002,28 @@
         <v>12</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>66</v>
-      </c>
       <c r="G3" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
@@ -1043,28 +1044,28 @@
         <v>13</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>69</v>
-      </c>
       <c r="F4" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
@@ -1085,28 +1086,28 @@
         <v>14</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="F5" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
@@ -1127,28 +1128,28 @@
         <v>15</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>75</v>
-      </c>
       <c r="F6" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
@@ -1169,28 +1170,28 @@
         <v>16</v>
       </c>
       <c r="B7" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>78</v>
-      </c>
       <c r="F7" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
@@ -1211,28 +1212,28 @@
         <v>17</v>
       </c>
       <c r="B8" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>81</v>
-      </c>
       <c r="F8" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
@@ -3555,28 +3556,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>56</v>
-      </c>
       <c r="G2" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -5835,9 +5836,9 @@
   </sheetPr>
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -5906,16 +5907,16 @@
         <v>31</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>5</v>
@@ -5948,16 +5949,16 @@
         <v>31</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>5</v>
@@ -5990,16 +5991,16 @@
         <v>31</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>5</v>
@@ -6032,16 +6033,16 @@
         <v>31</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>5</v>
@@ -6074,16 +6075,16 @@
         <v>31</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -6116,16 +6117,16 @@
         <v>31</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>5</v>
@@ -6158,16 +6159,16 @@
         <v>31</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>5</v>
@@ -6200,16 +6201,16 @@
         <v>31</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>5</v>
@@ -6242,16 +6243,16 @@
         <v>31</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>5</v>
@@ -6284,16 +6285,16 @@
         <v>31</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>5</v>
@@ -8468,7 +8469,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -8531,20 +8532,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="15"/>
+        <v>80</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="F2" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>5</v>

</xml_diff>